<commit_message>
Trying to make sets repeat
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -414,65 +414,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Deadlift</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Spoto BP 1c 1"</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>High pin squats (9)</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Weighed Pull-ups</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Hanging knee raises</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -483,115 +432,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Squat</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Bench</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Pin Press @ Chin</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Scott curls</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Barbell Skullcrushers</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Deadlift</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Spoto BP 1c 1"</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>High pin squats (9)</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Weighed Pull-ups</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Hanging knee raises</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>